<commit_message>
std_CF updated for calculation of CF items from cum. CF statements (WIP). Updated standardized_CF excel.
</commit_message>
<xml_diff>
--- a/data/standardized_cashflow.xlsx
+++ b/data/standardized_cashflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\GitHub\SEC_data_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2FF61D-402D-CC44-8819-BFE57A1ACD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1830FCA-D900-409B-BA3E-0F6877ACE421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18880" yWindow="6440" windowWidth="26060" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>df_Facts_us_gaap_references</t>
   </si>
@@ -77,9 +77,6 @@
     <t>(Operating Activities) Change in Accounts Payable</t>
   </si>
   <si>
-    <t>(Operating Activities) Change in Other Working Capital</t>
-  </si>
-  <si>
     <t>(Operating Activities) Deferred Income Tax</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>(Investing Activities) Proceeds from maturities of Marketable Securities and Investment</t>
   </si>
   <si>
-    <t>(Investing Activities) Gain (Losses) in Other Investing Activities</t>
-  </si>
-  <si>
     <t>(Financing Activities) Proceeds from Issuance of Stock</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
   </si>
   <si>
     <t>(Financing Activities) Payment of Debt</t>
-  </si>
-  <si>
-    <t>(Financing Activities) Impact of Stock Options and Other</t>
   </si>
   <si>
     <t>The current period expense charged against earnings on long-lived, physical assets not used in production, and which are not intended for resale, to allocate or recognize the cost of such assets over their useful lives; or to record the reduction in book value of an intangible asset over the benefit period of such asset; or to reflect consumption during the period of an asset that is not used in production.</t>
@@ -319,9 +310,6 @@
   </si>
   <si>
     <t>ProceedsFromDebtNetOfIssuanceCosts</t>
-  </si>
-  <si>
-    <t>Other impact from Operating, Investing, Financing Activities</t>
   </si>
   <si>
     <t>EffectOfExchangeRateOnCashCashEquivalentsRestrictedCashAndRestrictedCashEquivalents</t>
@@ -385,21 +373,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -416,22 +398,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -448,9 +419,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -460,12 +428,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -481,7 +449,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -777,21 +745,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="83.1640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="65.33203125" customWidth="1"/>
+    <col min="1" max="1" width="74.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="83.125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="65.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -803,7 +771,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -815,8 +783,8 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -827,212 +795,216 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>46</v>
+      <c r="B17" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="4" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="4" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
@@ -1040,235 +1012,205 @@
         <v>69</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="C24" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="B29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="7" t="s">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>58</v>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>94</v>
-      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Check total quarters summarize to equally distribute cash flow item over less than 4 quarters.
</commit_message>
<xml_diff>
--- a/data/standardized_cashflow.xlsx
+++ b/data/standardized_cashflow.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\GitHub\SEC_data_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1830FCA-D900-409B-BA3E-0F6877ACE421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F6D8B1-FB83-4FFE-A1F5-B36F938D4AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
   <si>
     <t>df_Facts_us_gaap_references</t>
   </si>
@@ -224,10 +227,6 @@
     <t>Amount of gain (loss) on sale or disposal of property, plant and equipment assets, including oil and gas property and timber property.</t>
   </si>
   <si>
-    <t>ProceedsFromSaleAndMaturityOfMarketableSecurities
-N</t>
-  </si>
-  <si>
     <t>The cash inflow associated with the aggregate amount received by the entity through sale or maturity of marketable securities (held-to-maturity or available-for-sale) during the period.</t>
   </si>
   <si>
@@ -252,9 +251,6 @@
     <t>ProceedsFromSaleAndMaturityOfMarketableSecurities</t>
   </si>
   <si>
-    <t>(Investing Activities) Proceeds from sale of Marketable Securities and Investment</t>
-  </si>
-  <si>
     <t>ProceedsFromMaturitiesPrepaymentsAndCallsOfAvailableForSaleSecurities</t>
   </si>
   <si>
@@ -279,9 +275,6 @@
     <t>The cash outflow to reacquire common stock during the period.</t>
   </si>
   <si>
-    <t>The cash inflow from the additional capital contribution to the entit</t>
-  </si>
-  <si>
     <t>ProceedsFromIssuanceOfCommonStock</t>
   </si>
   <si>
@@ -337,6 +330,12 @@
   </si>
   <si>
     <t>Amount of cash inflow (outflow) from operating activities, excluding discontinued operations. Operating activity cash flows include transactions, adjustments, and changes in value not defined as investing or financing activities.</t>
+  </si>
+  <si>
+    <t>The cash inflow from the additional capital contribution to the entity.</t>
+  </si>
+  <si>
+    <t>(Investing Activities) Proceeds from sale or maturity of Marketable Securities and Investment</t>
   </si>
 </sst>
 </file>
@@ -402,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,11 +424,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -841,13 +837,13 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -935,7 +931,7 @@
         <v>43</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -973,13 +969,13 @@
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>62</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -987,18 +983,18 @@
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>67</v>
@@ -1006,112 +1002,112 @@
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>72</v>
+      <c r="A25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>48</v>
+      <c r="A26" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>78</v>
+        <v>21</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>86</v>
+      <c r="A32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1119,70 +1115,64 @@
         <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>51</v>
+      <c r="A34" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>96</v>
-      </c>
+      <c r="A37" s="3"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1198,21 +1188,17 @@
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="4"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:C37" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP : exception for cumulative values. Added new line in excel for change in cash
</commit_message>
<xml_diff>
--- a/data/standardized_cashflow.xlsx
+++ b/data/standardized_cashflow.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\GitHub\SEC_data_analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F6D8B1-FB83-4FFE-A1F5-B36F938D4AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4FCAF3-750E-BB41-8E1E-37575B567F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20040" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
   <si>
     <t>df_Facts_us_gaap_references</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>(Investing Activities) Proceeds from sale or maturity of Marketable Securities and Investment</t>
+  </si>
+  <si>
+    <t>Amount of increase (decrease) in cash and cash equivalents. Cash and cash equivalents are the amount of currency on hand as well as demand deposits with banks or financial institutions. Includes other kinds of accounts that have the general characteristics of demand deposits. Also includes short-term, highly liquid investments that are both readily convertible to known amounts of cash and so near their maturity that they present insignificant risk of changes in value because of changes in interest rates. Includes effect from exchange rate changes.</t>
+  </si>
+  <si>
+    <t>CashAndCashEquivalentsPeriodIncreaseDecrease</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,7 +451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -741,21 +747,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="AC3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="74.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="83.125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="65.375" customWidth="1"/>
+    <col min="1" max="1" width="74.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="83.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -767,7 +773,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -779,7 +785,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -791,7 +797,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -802,7 +808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -813,7 +819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -824,7 +830,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -835,7 +841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -846,7 +852,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -857,7 +863,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -868,7 +874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -879,7 +885,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -890,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -901,7 +907,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -912,7 +918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -923,7 +929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
@@ -934,7 +940,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -945,7 +951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -956,7 +962,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -967,7 +973,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -978,7 +984,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
@@ -989,7 +995,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>98</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>48</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>75</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>21</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>79</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>79</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>89</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -1143,62 +1149,73 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="B45" s="3"/>
       <c r="C45" s="4"/>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C37" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}"/>
+  <autoFilter ref="A1:C38" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP : calculation of quarterly value and excel aggregate
Calculation of quarterly value fixed for cash flow. To check records where No. Missing Quarters is != 0 (exceptions). Also, excel file updated indicating quarterly val to aggregate.
</commit_message>
<xml_diff>
--- a/data/standardized_cashflow.xlsx
+++ b/data/standardized_cashflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4FCAF3-750E-BB41-8E1E-37575B567F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68C714A-3141-D744-A510-F46C7423D298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20040" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
   <si>
     <t>df_Facts_us_gaap_references</t>
   </si>
@@ -342,6 +342,21 @@
   </si>
   <si>
     <t>CashAndCashEquivalentsPeriodIncreaseDecrease</t>
+  </si>
+  <si>
+    <t>The increase (decrease) during the reporting period in the obligations due for goods and services provided by the following types of related parties: a parent company and its subsidiaries, subsidiaries of a common parent, an entity and trust for the benefit of employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entities' management, an entity and its principal owners, management, or member of their immediate families, affiliates, or other parties with the ability to exert significant influence.</t>
+  </si>
+  <si>
+    <t>IncreaseDecreaseInAccountsPayableRelatedParties</t>
+  </si>
+  <si>
+    <t>To Aggregate</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -747,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,6 +786,9 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -783,6 +801,9 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,6 +816,9 @@
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -807,6 +831,9 @@
       <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -818,6 +845,9 @@
       <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -829,6 +859,9 @@
       <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -840,6 +873,9 @@
       <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -851,6 +887,9 @@
       <c r="C8" s="7" t="s">
         <v>73</v>
       </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -862,360 +901,461 @@
       <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>33</v>
+        <v>102</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>35</v>
+      <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>40</v>
+      <c r="B12" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="D22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="D25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="D28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="4"/>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C38" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}"/>
+  <autoFilter ref="A1:C39" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>